<commit_message>
Update Fact sheets and paper
</commit_message>
<xml_diff>
--- a/doc/Aufnahmen/Fact_sheet_Hollow_Form_ID112.xlsx
+++ b/doc/Aufnahmen/Fact_sheet_Hollow_Form_ID112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CSeimn\Documents\edu\Envimaster-Geomorph\repo\doc\Aufnahmen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A1439B-7506-4619-80C7-C54ACAAD1D43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9D8DB7-F26B-49F2-A1FC-3BCDB5A396F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C11A25ED-35C3-41CF-904F-F9C2490EB3CC}"/>
   </bookViews>
@@ -64,12 +64,6 @@
   <si>
     <t>Anzahl 
 Schläge</t>
-  </si>
-  <si>
-    <t>Leerprobe</t>
-  </si>
-  <si>
-    <t>Schluffig</t>
   </si>
   <si>
     <t>Grundwasser</t>
@@ -153,6 +147,12 @@
   <si>
     <t>Fact_sheet_Hollow_Form_ID112</t>
   </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>leer</t>
+  </si>
 </sst>
 </file>
 
@@ -519,6 +519,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -603,15 +612,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:AE101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,54 +1007,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
+      <c r="A1" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="45" t="s">
+      <c r="A2" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="47"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="50"/>
       <c r="U2" s="26"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -1068,655 +1068,655 @@
       <c r="AE2" s="1"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="50"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="53"/>
       <c r="U3" s="26"/>
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="50"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="53"/>
       <c r="U4" s="26"/>
       <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="53"/>
       <c r="U5" s="26"/>
       <c r="V5" s="1"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="50"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="53"/>
       <c r="U6" s="26"/>
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="50"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="53"/>
       <c r="U7" s="26"/>
       <c r="V7" s="1"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="50"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="53"/>
       <c r="U8" s="26"/>
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="50"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="53"/>
       <c r="U9" s="26"/>
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="49"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="50"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="52"/>
+      <c r="T10" s="53"/>
       <c r="U10" s="26"/>
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="50"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="53"/>
       <c r="U11" s="26"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="50"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="53"/>
       <c r="U12" s="26"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="49"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="50"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
+      <c r="T13" s="53"/>
       <c r="U13" s="26"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="50"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="53"/>
       <c r="U14" s="26"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="50"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="53"/>
       <c r="U15" s="26"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="49"/>
-      <c r="R16" s="49"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="50"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="52"/>
+      <c r="T16" s="53"/>
       <c r="U16" s="26"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="49"/>
-      <c r="R17" s="49"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="50"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="52"/>
+      <c r="T17" s="53"/>
       <c r="U17" s="26"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="50"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="53"/>
       <c r="U18" s="26"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="50"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="53"/>
       <c r="U19" s="26"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="50"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="52"/>
+      <c r="R20" s="52"/>
+      <c r="S20" s="52"/>
+      <c r="T20" s="53"/>
       <c r="U20" s="26"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="50"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
+      <c r="T21" s="53"/>
       <c r="U21" s="26"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="50"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="52"/>
+      <c r="S22" s="52"/>
+      <c r="T22" s="53"/>
       <c r="U22" s="26"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="49"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="50"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="52"/>
+      <c r="T23" s="53"/>
       <c r="U23" s="26"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="49"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="50"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="52"/>
+      <c r="T24" s="53"/>
       <c r="U24" s="26"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49"/>
-      <c r="S25" s="49"/>
-      <c r="T25" s="50"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
+      <c r="T25" s="53"/>
       <c r="U25" s="26"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="50"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
+      <c r="T26" s="53"/>
       <c r="U26" s="26"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="50"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="52"/>
+      <c r="T27" s="53"/>
       <c r="U27" s="26"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="50"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="52"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="53"/>
       <c r="U28" s="26"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="50"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="52"/>
+      <c r="S29" s="52"/>
+      <c r="T29" s="53"/>
       <c r="U29" s="26"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-      <c r="P30" s="52"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="52"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="53"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="55"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="55"/>
+      <c r="T30" s="56"/>
       <c r="U30" s="26"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1731,7 +1731,7 @@
       <c r="D32" s="11"/>
       <c r="E32" s="10"/>
       <c r="F32" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1742,23 +1742,23 @@
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
-      <c r="F34" s="36" t="s">
+      <c r="F34" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="37"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="38"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="41"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -1766,21 +1766,21 @@
       <c r="C35" s="1"/>
       <c r="D35" s="8"/>
       <c r="E35" s="22"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="40"/>
-      <c r="Q35" s="40"/>
-      <c r="R35" s="40"/>
-      <c r="S35" s="40"/>
-      <c r="T35" s="41"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="43"/>
+      <c r="T35" s="44"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
@@ -1796,729 +1796,729 @@
         <v>3</v>
       </c>
       <c r="E36" s="22"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
-      <c r="P36" s="40"/>
-      <c r="Q36" s="40"/>
-      <c r="R36" s="40"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="41"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="43"/>
+      <c r="S36" s="43"/>
+      <c r="T36" s="44"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="28">
+        <v>7</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="43"/>
+      <c r="S37" s="43"/>
+      <c r="T37" s="44"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="28">
+        <v>5</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="43"/>
+      <c r="T38" s="44"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B39" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="56">
-        <v>7</v>
-      </c>
-      <c r="D37" s="19"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="O37" s="40"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="40"/>
-      <c r="R37" s="40"/>
-      <c r="S37" s="40"/>
-      <c r="T37" s="41"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+      <c r="C39" s="28">
+        <v>18</v>
+      </c>
+      <c r="D39" s="19"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+      <c r="P39" s="43"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="43"/>
+      <c r="S39" s="43"/>
+      <c r="T39" s="44"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B40" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="28">
+        <v>2</v>
+      </c>
+      <c r="D40" s="19"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="43"/>
+      <c r="T40" s="44"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="56">
+      <c r="C41" s="28">
+        <v>13</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="43"/>
+      <c r="S41" s="43"/>
+      <c r="T41" s="44"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="28">
+        <v>45</v>
+      </c>
+      <c r="D42" s="19"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+      <c r="P42" s="43"/>
+      <c r="Q42" s="43"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="44"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="28">
+        <v>70</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="43"/>
+      <c r="P43" s="43"/>
+      <c r="Q43" s="43"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="44"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="28">
+        <v>1</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="43"/>
+      <c r="P44" s="43"/>
+      <c r="Q44" s="43"/>
+      <c r="R44" s="43"/>
+      <c r="S44" s="43"/>
+      <c r="T44" s="44"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="28">
+        <v>10</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43"/>
+      <c r="O45" s="43"/>
+      <c r="P45" s="43"/>
+      <c r="Q45" s="43"/>
+      <c r="R45" s="43"/>
+      <c r="S45" s="43"/>
+      <c r="T45" s="44"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="28">
+        <v>89</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" s="42"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="43"/>
+      <c r="P46" s="43"/>
+      <c r="Q46" s="43"/>
+      <c r="R46" s="43"/>
+      <c r="S46" s="43"/>
+      <c r="T46" s="44"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="28">
         <v>5</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="40"/>
-      <c r="S38" s="40"/>
-      <c r="T38" s="41"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="56">
-        <v>18</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="40"/>
-      <c r="S39" s="40"/>
-      <c r="T39" s="41"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="56">
-        <v>2</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="40"/>
-      <c r="S40" s="40"/>
-      <c r="T40" s="41"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="56">
-        <v>13</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="O41" s="40"/>
-      <c r="P41" s="40"/>
-      <c r="Q41" s="40"/>
-      <c r="R41" s="40"/>
-      <c r="S41" s="40"/>
-      <c r="T41" s="41"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="56">
-        <v>45</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="40"/>
-      <c r="R42" s="40"/>
-      <c r="S42" s="40"/>
-      <c r="T42" s="41"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="56">
-        <v>70</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="39"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="40"/>
-      <c r="O43" s="40"/>
-      <c r="P43" s="40"/>
-      <c r="Q43" s="40"/>
-      <c r="R43" s="40"/>
-      <c r="S43" s="40"/>
-      <c r="T43" s="41"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="56">
-        <v>1</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="40"/>
-      <c r="O44" s="40"/>
-      <c r="P44" s="40"/>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="40"/>
-      <c r="S44" s="40"/>
-      <c r="T44" s="41"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="56">
-        <v>10</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="40"/>
-      <c r="P45" s="40"/>
-      <c r="Q45" s="40"/>
-      <c r="R45" s="40"/>
-      <c r="S45" s="40"/>
-      <c r="T45" s="41"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="D47" s="19"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="43"/>
+      <c r="P47" s="43"/>
+      <c r="Q47" s="43"/>
+      <c r="R47" s="43"/>
+      <c r="S47" s="43"/>
+      <c r="T47" s="44"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="56">
-        <v>89</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="39"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="40"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="40"/>
-      <c r="O46" s="40"/>
-      <c r="P46" s="40"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="40"/>
-      <c r="S46" s="40"/>
-      <c r="T46" s="41"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="56">
-        <v>5</v>
-      </c>
-      <c r="D47" s="19"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="40"/>
-      <c r="N47" s="40"/>
-      <c r="O47" s="40"/>
-      <c r="P47" s="40"/>
-      <c r="Q47" s="40"/>
-      <c r="R47" s="40"/>
-      <c r="S47" s="40"/>
-      <c r="T47" s="41"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="55" t="s">
-        <v>25</v>
-      </c>
       <c r="B48" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="56">
+        <v>35</v>
+      </c>
+      <c r="C48" s="28">
         <v>60</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="39"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="40"/>
-      <c r="N48" s="40"/>
-      <c r="O48" s="40"/>
-      <c r="P48" s="40"/>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="40"/>
-      <c r="S48" s="40"/>
-      <c r="T48" s="41"/>
+        <v>36</v>
+      </c>
+      <c r="F48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="43"/>
+      <c r="P48" s="43"/>
+      <c r="Q48" s="43"/>
+      <c r="R48" s="43"/>
+      <c r="S48" s="43"/>
+      <c r="T48" s="44"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="2"/>
       <c r="D49" s="13"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="40"/>
-      <c r="N49" s="40"/>
-      <c r="O49" s="40"/>
-      <c r="P49" s="40"/>
-      <c r="Q49" s="40"/>
-      <c r="R49" s="40"/>
-      <c r="S49" s="40"/>
-      <c r="T49" s="41"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="43"/>
+      <c r="O49" s="43"/>
+      <c r="P49" s="43"/>
+      <c r="Q49" s="43"/>
+      <c r="R49" s="43"/>
+      <c r="S49" s="43"/>
+      <c r="T49" s="44"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="2"/>
       <c r="D50" s="13"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40"/>
-      <c r="N50" s="40"/>
-      <c r="O50" s="40"/>
-      <c r="P50" s="40"/>
-      <c r="Q50" s="40"/>
-      <c r="R50" s="40"/>
-      <c r="S50" s="40"/>
-      <c r="T50" s="41"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="43"/>
+      <c r="O50" s="43"/>
+      <c r="P50" s="43"/>
+      <c r="Q50" s="43"/>
+      <c r="R50" s="43"/>
+      <c r="S50" s="43"/>
+      <c r="T50" s="44"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="2"/>
       <c r="D51" s="13"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
-      <c r="P51" s="40"/>
-      <c r="Q51" s="40"/>
-      <c r="R51" s="40"/>
-      <c r="S51" s="40"/>
-      <c r="T51" s="41"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
+      <c r="M51" s="43"/>
+      <c r="N51" s="43"/>
+      <c r="O51" s="43"/>
+      <c r="P51" s="43"/>
+      <c r="Q51" s="43"/>
+      <c r="R51" s="43"/>
+      <c r="S51" s="43"/>
+      <c r="T51" s="44"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="2"/>
       <c r="D52" s="13"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="40"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40"/>
-      <c r="N52" s="40"/>
-      <c r="O52" s="40"/>
-      <c r="P52" s="40"/>
-      <c r="Q52" s="40"/>
-      <c r="R52" s="40"/>
-      <c r="S52" s="40"/>
-      <c r="T52" s="41"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="43"/>
+      <c r="M52" s="43"/>
+      <c r="N52" s="43"/>
+      <c r="O52" s="43"/>
+      <c r="P52" s="43"/>
+      <c r="Q52" s="43"/>
+      <c r="R52" s="43"/>
+      <c r="S52" s="43"/>
+      <c r="T52" s="44"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="2"/>
       <c r="D53" s="13"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="40"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="40"/>
-      <c r="N53" s="40"/>
-      <c r="O53" s="40"/>
-      <c r="P53" s="40"/>
-      <c r="Q53" s="40"/>
-      <c r="R53" s="40"/>
-      <c r="S53" s="40"/>
-      <c r="T53" s="41"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
+      <c r="N53" s="43"/>
+      <c r="O53" s="43"/>
+      <c r="P53" s="43"/>
+      <c r="Q53" s="43"/>
+      <c r="R53" s="43"/>
+      <c r="S53" s="43"/>
+      <c r="T53" s="44"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="2"/>
       <c r="D54" s="13"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
-      <c r="O54" s="40"/>
-      <c r="P54" s="40"/>
-      <c r="Q54" s="40"/>
-      <c r="R54" s="40"/>
-      <c r="S54" s="40"/>
-      <c r="T54" s="41"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="43"/>
+      <c r="M54" s="43"/>
+      <c r="N54" s="43"/>
+      <c r="O54" s="43"/>
+      <c r="P54" s="43"/>
+      <c r="Q54" s="43"/>
+      <c r="R54" s="43"/>
+      <c r="S54" s="43"/>
+      <c r="T54" s="44"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="2"/>
       <c r="D55" s="13"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-      <c r="L55" s="40"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
-      <c r="O55" s="40"/>
-      <c r="P55" s="40"/>
-      <c r="Q55" s="40"/>
-      <c r="R55" s="40"/>
-      <c r="S55" s="40"/>
-      <c r="T55" s="41"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="43"/>
+      <c r="P55" s="43"/>
+      <c r="Q55" s="43"/>
+      <c r="R55" s="43"/>
+      <c r="S55" s="43"/>
+      <c r="T55" s="44"/>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="40"/>
-      <c r="K56" s="40"/>
-      <c r="L56" s="40"/>
-      <c r="M56" s="40"/>
-      <c r="N56" s="40"/>
-      <c r="O56" s="40"/>
-      <c r="P56" s="40"/>
-      <c r="Q56" s="40"/>
-      <c r="R56" s="40"/>
-      <c r="S56" s="40"/>
-      <c r="T56" s="41"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="43"/>
+      <c r="P56" s="43"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="43"/>
+      <c r="S56" s="43"/>
+      <c r="T56" s="44"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="2"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="40"/>
-      <c r="L57" s="40"/>
-      <c r="M57" s="40"/>
-      <c r="N57" s="40"/>
-      <c r="O57" s="40"/>
-      <c r="P57" s="40"/>
-      <c r="Q57" s="40"/>
-      <c r="R57" s="40"/>
-      <c r="S57" s="40"/>
-      <c r="T57" s="41"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="43"/>
+      <c r="Q57" s="43"/>
+      <c r="R57" s="43"/>
+      <c r="S57" s="43"/>
+      <c r="T57" s="44"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="2"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="40"/>
-      <c r="L58" s="40"/>
-      <c r="M58" s="40"/>
-      <c r="N58" s="40"/>
-      <c r="O58" s="40"/>
-      <c r="P58" s="40"/>
-      <c r="Q58" s="40"/>
-      <c r="R58" s="40"/>
-      <c r="S58" s="40"/>
-      <c r="T58" s="41"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
+      <c r="K58" s="43"/>
+      <c r="L58" s="43"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="43"/>
+      <c r="P58" s="43"/>
+      <c r="Q58" s="43"/>
+      <c r="R58" s="43"/>
+      <c r="S58" s="43"/>
+      <c r="T58" s="44"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="2"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="40"/>
-      <c r="L59" s="40"/>
-      <c r="M59" s="40"/>
-      <c r="N59" s="40"/>
-      <c r="O59" s="40"/>
-      <c r="P59" s="40"/>
-      <c r="Q59" s="40"/>
-      <c r="R59" s="40"/>
-      <c r="S59" s="40"/>
-      <c r="T59" s="41"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
+      <c r="J59" s="43"/>
+      <c r="K59" s="43"/>
+      <c r="L59" s="43"/>
+      <c r="M59" s="43"/>
+      <c r="N59" s="43"/>
+      <c r="O59" s="43"/>
+      <c r="P59" s="43"/>
+      <c r="Q59" s="43"/>
+      <c r="R59" s="43"/>
+      <c r="S59" s="43"/>
+      <c r="T59" s="44"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="2"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="40"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
-      <c r="P60" s="40"/>
-      <c r="Q60" s="40"/>
-      <c r="R60" s="40"/>
-      <c r="S60" s="40"/>
-      <c r="T60" s="41"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="43"/>
+      <c r="M60" s="43"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="43"/>
+      <c r="P60" s="43"/>
+      <c r="Q60" s="43"/>
+      <c r="R60" s="43"/>
+      <c r="S60" s="43"/>
+      <c r="T60" s="44"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="2"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="40"/>
-      <c r="K61" s="40"/>
-      <c r="L61" s="40"/>
-      <c r="M61" s="40"/>
-      <c r="N61" s="40"/>
-      <c r="O61" s="40"/>
-      <c r="P61" s="40"/>
-      <c r="Q61" s="40"/>
-      <c r="R61" s="40"/>
-      <c r="S61" s="40"/>
-      <c r="T61" s="41"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
+      <c r="K61" s="43"/>
+      <c r="L61" s="43"/>
+      <c r="M61" s="43"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
+      <c r="P61" s="43"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
+      <c r="S61" s="43"/>
+      <c r="T61" s="44"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
       <c r="D62" s="2"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-      <c r="J62" s="40"/>
-      <c r="K62" s="40"/>
-      <c r="L62" s="40"/>
-      <c r="M62" s="40"/>
-      <c r="N62" s="40"/>
-      <c r="O62" s="40"/>
-      <c r="P62" s="40"/>
-      <c r="Q62" s="40"/>
-      <c r="R62" s="40"/>
-      <c r="S62" s="40"/>
-      <c r="T62" s="41"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
+      <c r="J62" s="43"/>
+      <c r="K62" s="43"/>
+      <c r="L62" s="43"/>
+      <c r="M62" s="43"/>
+      <c r="N62" s="43"/>
+      <c r="O62" s="43"/>
+      <c r="P62" s="43"/>
+      <c r="Q62" s="43"/>
+      <c r="R62" s="43"/>
+      <c r="S62" s="43"/>
+      <c r="T62" s="44"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
       <c r="D63" s="2"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
-      <c r="L63" s="40"/>
-      <c r="M63" s="40"/>
-      <c r="N63" s="40"/>
-      <c r="O63" s="40"/>
-      <c r="P63" s="40"/>
-      <c r="Q63" s="40"/>
-      <c r="R63" s="40"/>
-      <c r="S63" s="40"/>
-      <c r="T63" s="41"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="43"/>
+      <c r="L63" s="43"/>
+      <c r="M63" s="43"/>
+      <c r="N63" s="43"/>
+      <c r="O63" s="43"/>
+      <c r="P63" s="43"/>
+      <c r="Q63" s="43"/>
+      <c r="R63" s="43"/>
+      <c r="S63" s="43"/>
+      <c r="T63" s="44"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="2"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="40"/>
-      <c r="K64" s="40"/>
-      <c r="L64" s="40"/>
-      <c r="M64" s="40"/>
-      <c r="N64" s="40"/>
-      <c r="O64" s="40"/>
-      <c r="P64" s="40"/>
-      <c r="Q64" s="40"/>
-      <c r="R64" s="40"/>
-      <c r="S64" s="40"/>
-      <c r="T64" s="41"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="43"/>
+      <c r="K64" s="43"/>
+      <c r="L64" s="43"/>
+      <c r="M64" s="43"/>
+      <c r="N64" s="43"/>
+      <c r="O64" s="43"/>
+      <c r="P64" s="43"/>
+      <c r="Q64" s="43"/>
+      <c r="R64" s="43"/>
+      <c r="S64" s="43"/>
+      <c r="T64" s="44"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="2"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="40"/>
-      <c r="K65" s="40"/>
-      <c r="L65" s="40"/>
-      <c r="M65" s="40"/>
-      <c r="N65" s="40"/>
-      <c r="O65" s="40"/>
-      <c r="P65" s="40"/>
-      <c r="Q65" s="40"/>
-      <c r="R65" s="40"/>
-      <c r="S65" s="40"/>
-      <c r="T65" s="41"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
+      <c r="J65" s="43"/>
+      <c r="K65" s="43"/>
+      <c r="L65" s="43"/>
+      <c r="M65" s="43"/>
+      <c r="N65" s="43"/>
+      <c r="O65" s="43"/>
+      <c r="P65" s="43"/>
+      <c r="Q65" s="43"/>
+      <c r="R65" s="43"/>
+      <c r="S65" s="43"/>
+      <c r="T65" s="44"/>
     </row>
     <row r="66" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
       <c r="D66" s="3"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
-      <c r="J66" s="43"/>
-      <c r="K66" s="43"/>
-      <c r="L66" s="43"/>
-      <c r="M66" s="43"/>
-      <c r="N66" s="43"/>
-      <c r="O66" s="43"/>
-      <c r="P66" s="43"/>
-      <c r="Q66" s="43"/>
-      <c r="R66" s="43"/>
-      <c r="S66" s="43"/>
-      <c r="T66" s="44"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="46"/>
+      <c r="M66" s="46"/>
+      <c r="N66" s="46"/>
+      <c r="O66" s="46"/>
+      <c r="P66" s="46"/>
+      <c r="Q66" s="46"/>
+      <c r="R66" s="46"/>
+      <c r="S66" s="46"/>
+      <c r="T66" s="47"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G67" s="1"/>
@@ -2672,7 +2672,7 @@
       <c r="B72" s="19">
         <v>18</v>
       </c>
-      <c r="C72" s="56"/>
+      <c r="C72" s="28"/>
       <c r="D72" s="19">
         <v>10</v>
       </c>
@@ -2687,21 +2687,21 @@
       <c r="I72" s="19">
         <v>8</v>
       </c>
-      <c r="J72" s="56"/>
+      <c r="J72" s="28"/>
       <c r="K72" s="19">
         <v>10</v>
       </c>
       <c r="L72" s="19">
         <v>7</v>
       </c>
-      <c r="M72" s="56"/>
+      <c r="M72" s="28"/>
       <c r="O72" s="19">
         <v>10</v>
       </c>
       <c r="P72" s="19">
         <v>10</v>
       </c>
-      <c r="Q72" s="56"/>
+      <c r="Q72" s="28"/>
       <c r="R72" s="19">
         <v>10</v>
       </c>
@@ -2715,7 +2715,7 @@
       <c r="B73" s="19">
         <v>17</v>
       </c>
-      <c r="C73" s="56"/>
+      <c r="C73" s="28"/>
       <c r="D73" s="19">
         <v>20</v>
       </c>
@@ -2730,21 +2730,21 @@
       <c r="I73" s="19">
         <v>10</v>
       </c>
-      <c r="J73" s="56"/>
+      <c r="J73" s="28"/>
       <c r="K73" s="19">
         <v>20</v>
       </c>
       <c r="L73" s="19">
         <v>6</v>
       </c>
-      <c r="M73" s="56"/>
+      <c r="M73" s="28"/>
       <c r="O73" s="19">
         <v>20</v>
       </c>
       <c r="P73" s="19">
         <v>15</v>
       </c>
-      <c r="Q73" s="56"/>
+      <c r="Q73" s="28"/>
       <c r="R73" s="19">
         <v>20</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="B74" s="19">
         <v>18</v>
       </c>
-      <c r="C74" s="56"/>
+      <c r="C74" s="28"/>
       <c r="D74" s="19">
         <v>30</v>
       </c>
@@ -2773,21 +2773,21 @@
       <c r="I74" s="19">
         <v>13</v>
       </c>
-      <c r="J74" s="56"/>
+      <c r="J74" s="28"/>
       <c r="K74" s="19">
         <v>30</v>
       </c>
       <c r="L74" s="19">
         <v>12</v>
       </c>
-      <c r="M74" s="56"/>
+      <c r="M74" s="28"/>
       <c r="O74" s="19">
         <v>30</v>
       </c>
       <c r="P74" s="19">
         <v>15</v>
       </c>
-      <c r="Q74" s="56"/>
+      <c r="Q74" s="28"/>
       <c r="R74" s="19">
         <v>30</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="B75" s="19">
         <v>18</v>
       </c>
-      <c r="C75" s="56"/>
+      <c r="C75" s="28"/>
       <c r="D75" s="19">
         <v>40</v>
       </c>
@@ -2816,21 +2816,21 @@
       <c r="I75" s="19">
         <v>7</v>
       </c>
-      <c r="J75" s="56"/>
+      <c r="J75" s="28"/>
       <c r="K75" s="19">
         <v>40</v>
       </c>
       <c r="L75" s="19">
         <v>14</v>
       </c>
-      <c r="M75" s="56"/>
+      <c r="M75" s="28"/>
       <c r="O75" s="19">
         <v>40</v>
       </c>
       <c r="P75" s="19">
         <v>14</v>
       </c>
-      <c r="Q75" s="56"/>
+      <c r="Q75" s="28"/>
       <c r="R75" s="19">
         <v>40</v>
       </c>
@@ -2844,7 +2844,7 @@
       <c r="B76" s="19">
         <v>17</v>
       </c>
-      <c r="C76" s="56"/>
+      <c r="C76" s="28"/>
       <c r="D76" s="19">
         <v>50</v>
       </c>
@@ -2859,21 +2859,21 @@
       <c r="I76" s="19">
         <v>8</v>
       </c>
-      <c r="J76" s="56"/>
+      <c r="J76" s="28"/>
       <c r="K76" s="19">
         <v>50</v>
       </c>
       <c r="L76" s="19">
         <v>19</v>
       </c>
-      <c r="M76" s="56"/>
+      <c r="M76" s="28"/>
       <c r="O76" s="19">
         <v>50</v>
       </c>
       <c r="P76" s="19">
         <v>13</v>
       </c>
-      <c r="Q76" s="56"/>
+      <c r="Q76" s="28"/>
       <c r="R76" s="19">
         <v>50</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="B77" s="19">
         <v>39</v>
       </c>
-      <c r="C77" s="56"/>
+      <c r="C77" s="28"/>
       <c r="D77" s="19">
         <v>60</v>
       </c>
@@ -2901,21 +2901,21 @@
       <c r="I77" s="19">
         <v>12</v>
       </c>
-      <c r="J77" s="56"/>
+      <c r="J77" s="28"/>
       <c r="K77" s="19">
         <v>60</v>
       </c>
       <c r="L77" s="19">
         <v>22</v>
       </c>
-      <c r="M77" s="56"/>
+      <c r="M77" s="28"/>
       <c r="O77" s="19">
         <v>60</v>
       </c>
       <c r="P77" s="19">
         <v>10</v>
       </c>
-      <c r="Q77" s="56"/>
+      <c r="Q77" s="28"/>
       <c r="R77" s="19">
         <v>60</v>
       </c>
@@ -2927,8 +2927,8 @@
         <v>70</v>
       </c>
       <c r="B78" s="19"/>
-      <c r="C78" s="57" t="s">
-        <v>30</v>
+      <c r="C78" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="D78" s="19">
         <v>70</v>
@@ -2943,21 +2943,21 @@
       <c r="I78" s="19">
         <v>9</v>
       </c>
-      <c r="J78" s="56"/>
+      <c r="J78" s="28"/>
       <c r="K78" s="19">
         <v>70</v>
       </c>
       <c r="L78" s="19">
         <v>22</v>
       </c>
-      <c r="M78" s="56"/>
+      <c r="M78" s="28"/>
       <c r="O78" s="19">
         <v>70</v>
       </c>
       <c r="P78" s="19">
         <v>9</v>
       </c>
-      <c r="Q78" s="56"/>
+      <c r="Q78" s="28"/>
       <c r="R78" s="19">
         <v>70</v>
       </c>
@@ -2981,21 +2981,21 @@
       <c r="I79" s="19">
         <v>15</v>
       </c>
-      <c r="J79" s="56"/>
+      <c r="J79" s="28"/>
       <c r="K79" s="19">
         <v>80</v>
       </c>
       <c r="L79" s="19">
         <v>15</v>
       </c>
-      <c r="M79" s="56"/>
+      <c r="M79" s="28"/>
       <c r="O79" s="19">
         <v>80</v>
       </c>
       <c r="P79" s="19">
         <v>7</v>
       </c>
-      <c r="Q79" s="56"/>
+      <c r="Q79" s="28"/>
       <c r="R79" s="19">
         <v>80</v>
       </c>
@@ -3019,21 +3019,21 @@
       <c r="I80" s="19">
         <v>16</v>
       </c>
-      <c r="J80" s="56"/>
+      <c r="J80" s="28"/>
       <c r="K80" s="19">
         <v>90</v>
       </c>
       <c r="L80" s="19">
         <v>15</v>
       </c>
-      <c r="M80" s="56"/>
+      <c r="M80" s="28"/>
       <c r="O80" s="19">
         <v>90</v>
       </c>
       <c r="P80" s="19">
         <v>6</v>
       </c>
-      <c r="Q80" s="56"/>
+      <c r="Q80" s="28"/>
       <c r="R80" s="19">
         <v>90</v>
       </c>
@@ -3057,21 +3057,21 @@
       <c r="I81" s="19">
         <v>18</v>
       </c>
-      <c r="J81" s="56"/>
+      <c r="J81" s="28"/>
       <c r="K81" s="19">
         <v>100</v>
       </c>
       <c r="L81" s="19">
         <v>14</v>
       </c>
-      <c r="M81" s="56"/>
+      <c r="M81" s="28"/>
       <c r="O81" s="19">
         <v>100</v>
       </c>
       <c r="P81" s="19">
         <v>7</v>
       </c>
-      <c r="Q81" s="56"/>
+      <c r="Q81" s="28"/>
       <c r="R81" s="19">
         <v>100</v>
       </c>
@@ -3095,21 +3095,21 @@
       <c r="I82" s="19">
         <v>23</v>
       </c>
-      <c r="J82" s="56"/>
+      <c r="J82" s="28"/>
       <c r="K82" s="19">
         <v>110</v>
       </c>
       <c r="L82" s="19">
         <v>11</v>
       </c>
-      <c r="M82" s="56"/>
+      <c r="M82" s="28"/>
       <c r="O82" s="19">
         <v>110</v>
       </c>
       <c r="P82" s="19">
         <v>13</v>
       </c>
-      <c r="Q82" s="56"/>
+      <c r="Q82" s="28"/>
       <c r="R82" s="19">
         <v>110</v>
       </c>
@@ -3133,22 +3133,22 @@
       <c r="I83" s="19">
         <v>37</v>
       </c>
-      <c r="J83" s="56"/>
+      <c r="J83" s="28"/>
       <c r="K83" s="19">
         <v>120</v>
       </c>
       <c r="L83" s="19">
         <v>12</v>
       </c>
-      <c r="M83" s="56"/>
+      <c r="M83" s="28"/>
       <c r="O83" s="19">
         <v>120</v>
       </c>
       <c r="P83" s="19">
         <v>10</v>
       </c>
-      <c r="Q83" s="56" t="s">
-        <v>13</v>
+      <c r="Q83" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="R83" s="19">
         <v>120</v>
@@ -3173,15 +3173,15 @@
       <c r="I84" s="19">
         <v>46</v>
       </c>
-      <c r="J84" s="56"/>
+      <c r="J84" s="28"/>
       <c r="K84" s="19">
         <v>130</v>
       </c>
       <c r="L84" s="19">
         <v>7</v>
       </c>
-      <c r="M84" s="56" t="s">
-        <v>13</v>
+      <c r="M84" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="O84" s="19">
         <v>130</v>
@@ -3189,7 +3189,7 @@
       <c r="P84" s="19">
         <v>8</v>
       </c>
-      <c r="Q84" s="56"/>
+      <c r="Q84" s="28"/>
       <c r="R84" s="19">
         <v>130</v>
       </c>
@@ -3213,21 +3213,21 @@
       <c r="I85" s="19">
         <v>52</v>
       </c>
-      <c r="J85" s="56"/>
+      <c r="J85" s="28"/>
       <c r="K85" s="19">
         <v>140</v>
       </c>
       <c r="L85" s="19">
         <v>9</v>
       </c>
-      <c r="M85" s="56"/>
+      <c r="M85" s="28"/>
       <c r="O85" s="19">
         <v>140</v>
       </c>
       <c r="P85" s="19">
         <v>6</v>
       </c>
-      <c r="Q85" s="56"/>
+      <c r="Q85" s="28"/>
       <c r="R85" s="19">
         <v>140</v>
       </c>
@@ -3251,21 +3251,21 @@
       <c r="I86" s="19">
         <v>38</v>
       </c>
-      <c r="J86" s="56"/>
+      <c r="J86" s="28"/>
       <c r="K86" s="19">
         <v>150</v>
       </c>
       <c r="L86" s="19">
         <v>4</v>
       </c>
-      <c r="M86" s="56"/>
+      <c r="M86" s="28"/>
       <c r="O86" s="19">
         <v>150</v>
       </c>
       <c r="P86" s="19">
         <v>7</v>
       </c>
-      <c r="Q86" s="56"/>
+      <c r="Q86" s="28"/>
       <c r="R86" s="19">
         <v>150</v>
       </c>
@@ -3289,8 +3289,8 @@
       <c r="I87" s="19">
         <v>53</v>
       </c>
-      <c r="J87" s="57" t="s">
-        <v>31</v>
+      <c r="J87" s="29" t="s">
+        <v>29</v>
       </c>
       <c r="K87" s="19">
         <v>160</v>
@@ -3298,15 +3298,15 @@
       <c r="L87" s="19">
         <v>3</v>
       </c>
-      <c r="M87" s="56"/>
+      <c r="M87" s="28"/>
       <c r="O87" s="19">
         <v>160</v>
       </c>
       <c r="P87" s="19">
         <v>17</v>
       </c>
-      <c r="Q87" s="57" t="s">
-        <v>33</v>
+      <c r="Q87" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="R87" s="19">
         <v>160</v>
@@ -3336,7 +3336,7 @@
       <c r="L88" s="19">
         <v>4</v>
       </c>
-      <c r="M88" s="56"/>
+      <c r="M88" s="28"/>
       <c r="O88" s="19">
         <v>170</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="L89" s="19">
         <v>5</v>
       </c>
-      <c r="M89" s="56"/>
+      <c r="M89" s="28"/>
       <c r="O89" s="19">
         <v>180</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="L90" s="19">
         <v>4</v>
       </c>
-      <c r="M90" s="56"/>
+      <c r="M90" s="28"/>
       <c r="O90" s="19">
         <v>190</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="L91" s="19">
         <v>5</v>
       </c>
-      <c r="M91" s="56"/>
+      <c r="M91" s="28"/>
       <c r="O91" s="19">
         <v>200</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="L92" s="19">
         <v>8</v>
       </c>
-      <c r="M92" s="56"/>
+      <c r="M92" s="28"/>
       <c r="O92" s="19">
         <v>210</v>
       </c>
@@ -3506,7 +3506,7 @@
       <c r="L93" s="19">
         <v>10</v>
       </c>
-      <c r="M93" s="56"/>
+      <c r="M93" s="28"/>
       <c r="O93" s="19">
         <v>220</v>
       </c>
@@ -3540,7 +3540,7 @@
       <c r="L94" s="19">
         <v>11</v>
       </c>
-      <c r="M94" s="56"/>
+      <c r="M94" s="28"/>
       <c r="O94" s="19">
         <v>230</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="L95" s="19">
         <v>21</v>
       </c>
-      <c r="M95" s="56"/>
+      <c r="M95" s="28"/>
       <c r="O95" s="19">
         <v>240</v>
       </c>
@@ -3608,8 +3608,8 @@
       <c r="L96" s="19">
         <v>64</v>
       </c>
-      <c r="M96" s="57" t="s">
-        <v>32</v>
+      <c r="M96" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="O96" s="19">
         <v>250</v>

</xml_diff>